<commit_message>
Remove pi header from BOM.
</commit_message>
<xml_diff>
--- a/CAM_Outputs/MAINBOARD/BOM/PrintNC_GRBLHAL_Breakout_CAM_OUTPUT_A6.xlsx
+++ b/CAM_Outputs/MAINBOARD/BOM/PrintNC_GRBLHAL_Breakout_CAM_OUTPUT_A6.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repo\grblhal_2000_PrintNC\Project Outputs for PrintNC_GRBLHAL_Breakout\PrintNC_GRBLHAL_Breakout_UPLOAD_GERBERS_A6\BOM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repo\grblhal_2000_PrintNC\CAM_Outputs\MAINBOARD\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="280">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="275">
   <si>
     <t>Comment</t>
   </si>
@@ -45,21 +45,6 @@
   </si>
   <si>
     <t>Quantity</t>
-  </si>
-  <si>
-    <t>ADA3708</t>
-  </si>
-  <si>
-    <t>Raspberry Pi Zero WH _Zero W with Headers_</t>
-  </si>
-  <si>
-    <t>A1</t>
-  </si>
-  <si>
-    <t>ADA3708_RPI-ZERO</t>
-  </si>
-  <si>
-    <t>C50982</t>
   </si>
   <si>
     <t>100nF</t>
@@ -1209,9 +1194,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F70"/>
+  <dimension ref="A1:F69"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1257,7 +1244,7 @@
         <v>10</v>
       </c>
       <c r="F2" s="1">
-        <v>1</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1265,196 +1252,196 @@
         <v>11</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>15</v>
-      </c>
       <c r="F3" s="1">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="2" t="s">
+      <c r="E4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>19</v>
-      </c>
       <c r="F4" s="1">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="F5" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="2" t="s">
+      <c r="E6" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>25</v>
-      </c>
       <c r="F6" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>29</v>
-      </c>
       <c r="F7" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="C8" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D8" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>31</v>
-      </c>
       <c r="F8" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="D9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>35</v>
-      </c>
       <c r="F9" s="1">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F10" s="1">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F11" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E12" s="2" t="s">
         <v>41</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>43</v>
       </c>
       <c r="F12" s="1">
         <v>1</v>
@@ -1462,19 +1449,19 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13" s="2" t="s">
         <v>44</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>46</v>
       </c>
       <c r="F13" s="1">
         <v>1</v>
@@ -1482,22 +1469,22 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C14" s="2" t="s">
+      <c r="D14" s="2" t="s">
         <v>48</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>14</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>49</v>
       </c>
       <c r="F14" s="1">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -1505,56 +1492,56 @@
         <v>50</v>
       </c>
       <c r="B15" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="D15" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E15" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="D15" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>54</v>
-      </c>
       <c r="F15" s="1">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E16" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B16" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>57</v>
-      </c>
       <c r="F16" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E17" s="2" t="s">
         <v>58</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>60</v>
       </c>
       <c r="F17" s="1">
         <v>1</v>
@@ -1562,22 +1549,22 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C18" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="B18" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C18" s="2" t="s">
+      <c r="D18" s="2" t="s">
         <v>62</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>53</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>63</v>
       </c>
       <c r="F18" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -1585,27 +1572,27 @@
         <v>64</v>
       </c>
       <c r="B19" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C19" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="D19" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="E19" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="E19" s="2" t="s">
-        <v>68</v>
-      </c>
       <c r="F19" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>69</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>51</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>70</v>
@@ -1617,7 +1604,7 @@
         <v>72</v>
       </c>
       <c r="F20" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -1625,16 +1612,16 @@
         <v>73</v>
       </c>
       <c r="B21" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C21" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="D21" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E21" s="2" t="s">
         <v>75</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>77</v>
       </c>
       <c r="F21" s="1">
         <v>1</v>
@@ -1642,19 +1629,19 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E22" s="2" t="s">
         <v>78</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>80</v>
       </c>
       <c r="F22" s="1">
         <v>1</v>
@@ -1662,16 +1649,16 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C23" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="B23" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C23" s="2" t="s">
+      <c r="D23" s="2" t="s">
         <v>82</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>71</v>
       </c>
       <c r="E23" s="2" t="s">
         <v>83</v>
@@ -1705,16 +1692,16 @@
         <v>89</v>
       </c>
       <c r="B25" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C25" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="D25" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="E25" s="2" t="s">
         <v>91</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>93</v>
       </c>
       <c r="F25" s="1">
         <v>1</v>
@@ -1722,22 +1709,22 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C26" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="B26" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="C26" s="2" t="s">
+      <c r="D26" s="2" t="s">
         <v>95</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>87</v>
       </c>
       <c r="E26" s="2" t="s">
         <v>96</v>
       </c>
       <c r="F26" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -1751,10 +1738,10 @@
         <v>99</v>
       </c>
       <c r="D27" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="E27" s="2" t="s">
         <v>100</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>101</v>
       </c>
       <c r="F27" s="1">
         <v>2</v>
@@ -1762,42 +1749,42 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B28" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="C28" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="D28" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E28" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="D28" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="E28" s="2" t="s">
-        <v>105</v>
-      </c>
       <c r="F28" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B29" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="C29" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="C29" s="2" t="s">
+      <c r="D29" s="2" t="s">
         <v>108</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>28</v>
       </c>
       <c r="E29" s="2" t="s">
         <v>109</v>
       </c>
       <c r="F29" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -1817,7 +1804,7 @@
         <v>114</v>
       </c>
       <c r="F30" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -1837,7 +1824,7 @@
         <v>119</v>
       </c>
       <c r="F31" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
@@ -1857,7 +1844,7 @@
         <v>124</v>
       </c>
       <c r="F32" s="1">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -1877,7 +1864,7 @@
         <v>129</v>
       </c>
       <c r="F33" s="1">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
@@ -1894,30 +1881,30 @@
         <v>133</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="F34" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="B35" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="C35" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="C35" s="2" t="s">
+      <c r="D35" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="D35" s="2" t="s">
+      <c r="E35" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="E35" s="2" t="s">
-        <v>135</v>
-      </c>
       <c r="F35" s="1">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
@@ -1937,7 +1924,7 @@
         <v>143</v>
       </c>
       <c r="F36" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
@@ -1957,7 +1944,7 @@
         <v>148</v>
       </c>
       <c r="F37" s="1">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
@@ -1997,7 +1984,7 @@
         <v>158</v>
       </c>
       <c r="F39" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
@@ -2017,7 +2004,7 @@
         <v>163</v>
       </c>
       <c r="F40" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
@@ -2037,7 +2024,7 @@
         <v>168</v>
       </c>
       <c r="F41" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
@@ -2057,7 +2044,7 @@
         <v>173</v>
       </c>
       <c r="F42" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
@@ -2071,33 +2058,33 @@
         <v>176</v>
       </c>
       <c r="D43" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="E43" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="E43" s="2" t="s">
-        <v>178</v>
-      </c>
       <c r="F43" s="1">
-        <v>1</v>
+        <v>23</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="B44" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="B44" s="2" t="s">
+      <c r="C44" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="C44" s="2" t="s">
+      <c r="D44" s="2" t="s">
         <v>181</v>
-      </c>
-      <c r="D44" s="2" t="s">
-        <v>100</v>
       </c>
       <c r="E44" s="2" t="s">
         <v>182</v>
       </c>
       <c r="F44" s="1">
-        <v>23</v>
+        <v>3</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
@@ -2105,216 +2092,216 @@
         <v>183</v>
       </c>
       <c r="B45" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="C45" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="C45" s="2" t="s">
+      <c r="D45" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="E45" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="D45" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="E45" s="2" t="s">
-        <v>187</v>
-      </c>
       <c r="F45" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="E46" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="B46" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="C46" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="D46" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="E46" s="2" t="s">
-        <v>190</v>
-      </c>
       <c r="F46" s="1">
-        <v>2</v>
+        <v>14</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="E47" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="B47" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="C47" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="D47" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="E47" s="2" t="s">
-        <v>193</v>
-      </c>
       <c r="F47" s="1">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="E48" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="B48" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="C48" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="D48" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="E48" s="2" t="s">
-        <v>196</v>
-      </c>
       <c r="F48" s="1">
-        <v>15</v>
+        <v>35</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="E49" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="B49" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="C49" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="D49" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="E49" s="2" t="s">
-        <v>199</v>
-      </c>
       <c r="F49" s="1">
-        <v>35</v>
+        <v>8</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="E50" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="B50" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="C50" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="D50" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="E50" s="2" t="s">
-        <v>202</v>
-      </c>
       <c r="F50" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="E51" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="B51" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="C51" s="2" t="s">
-        <v>204</v>
-      </c>
-      <c r="D51" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="E51" s="2" t="s">
-        <v>205</v>
-      </c>
       <c r="F51" s="1">
-        <v>7</v>
+        <v>15</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="E52" s="2" t="s">
         <v>206</v>
       </c>
-      <c r="B52" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="C52" s="2" t="s">
-        <v>207</v>
-      </c>
-      <c r="D52" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="E52" s="2" t="s">
-        <v>208</v>
-      </c>
       <c r="F52" s="1">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="E53" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="B53" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="C53" s="2" t="s">
-        <v>210</v>
-      </c>
-      <c r="D53" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="E53" s="2" t="s">
-        <v>211</v>
-      </c>
       <c r="F53" s="1">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="E54" s="2" t="s">
         <v>212</v>
       </c>
-      <c r="B54" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="C54" s="2" t="s">
-        <v>213</v>
-      </c>
-      <c r="D54" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="E54" s="2" t="s">
-        <v>214</v>
-      </c>
       <c r="F54" s="1">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="E55" s="2" t="s">
         <v>215</v>
-      </c>
-      <c r="B55" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="C55" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="D55" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="E55" s="2" t="s">
-        <v>217</v>
       </c>
       <c r="F55" s="1">
         <v>1</v>
@@ -2322,19 +2309,19 @@
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="D56" s="2" t="s">
         <v>218</v>
       </c>
-      <c r="B56" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="C56" s="2" t="s">
+      <c r="E56" s="2" t="s">
         <v>219</v>
-      </c>
-      <c r="D56" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="E56" s="2" t="s">
-        <v>220</v>
       </c>
       <c r="F56" s="1">
         <v>1</v>
@@ -2342,19 +2329,19 @@
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="C57" s="2" t="s">
         <v>221</v>
       </c>
-      <c r="B57" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="C57" s="2" t="s">
+      <c r="D57" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="E57" s="2" t="s">
         <v>222</v>
-      </c>
-      <c r="D57" s="2" t="s">
-        <v>223</v>
-      </c>
-      <c r="E57" s="2" t="s">
-        <v>224</v>
       </c>
       <c r="F57" s="1">
         <v>1</v>
@@ -2362,19 +2349,19 @@
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="E58" s="2" t="s">
         <v>225</v>
-      </c>
-      <c r="B58" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="C58" s="2" t="s">
-        <v>226</v>
-      </c>
-      <c r="D58" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="E58" s="2" t="s">
-        <v>227</v>
       </c>
       <c r="F58" s="1">
         <v>1</v>
@@ -2382,42 +2369,42 @@
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="E59" s="2" t="s">
         <v>228</v>
       </c>
-      <c r="B59" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="C59" s="2" t="s">
-        <v>229</v>
-      </c>
-      <c r="D59" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="E59" s="2" t="s">
-        <v>230</v>
-      </c>
       <c r="F59" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="C60" s="2" t="s">
         <v>231</v>
       </c>
-      <c r="B60" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="C60" s="2" t="s">
+      <c r="D60" s="2" t="s">
         <v>232</v>
-      </c>
-      <c r="D60" s="2" t="s">
-        <v>128</v>
       </c>
       <c r="E60" s="2" t="s">
         <v>233</v>
       </c>
       <c r="F60" s="1">
-        <v>2</v>
+        <v>15</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
@@ -2437,7 +2424,7 @@
         <v>238</v>
       </c>
       <c r="F61" s="1">
-        <v>15</v>
+        <v>1</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
@@ -2511,10 +2498,10 @@
         <v>256</v>
       </c>
       <c r="D65" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="E65" s="2" t="s">
         <v>257</v>
-      </c>
-      <c r="E65" s="2" t="s">
-        <v>258</v>
       </c>
       <c r="F65" s="1">
         <v>1</v>
@@ -2522,19 +2509,19 @@
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="B66" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="B66" s="2" t="s">
+      <c r="C66" s="2" t="s">
         <v>260</v>
-      </c>
-      <c r="C66" s="2" t="s">
-        <v>261</v>
       </c>
       <c r="D66" s="2" t="s">
         <v>242</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="F66" s="1">
         <v>1</v>
@@ -2542,19 +2529,19 @@
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="B67" s="2" t="s">
         <v>263</v>
       </c>
-      <c r="B67" s="2" t="s">
+      <c r="C67" s="2" t="s">
         <v>264</v>
       </c>
-      <c r="C67" s="2" t="s">
+      <c r="D67" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="E67" s="2" t="s">
         <v>265</v>
-      </c>
-      <c r="D67" s="2" t="s">
-        <v>247</v>
-      </c>
-      <c r="E67" s="2" t="s">
-        <v>266</v>
       </c>
       <c r="F67" s="1">
         <v>1</v>
@@ -2562,19 +2549,19 @@
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="B68" s="2" t="s">
         <v>267</v>
       </c>
-      <c r="B68" s="2" t="s">
+      <c r="C68" s="2" t="s">
         <v>268</v>
       </c>
-      <c r="C68" s="2" t="s">
+      <c r="D68" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="E68" s="2" t="s">
         <v>269</v>
-      </c>
-      <c r="D68" s="2" t="s">
-        <v>242</v>
-      </c>
-      <c r="E68" s="2" t="s">
-        <v>270</v>
       </c>
       <c r="F68" s="1">
         <v>1</v>
@@ -2582,41 +2569,21 @@
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="B69" s="2" t="s">
         <v>271</v>
       </c>
-      <c r="B69" s="2" t="s">
+      <c r="C69" s="2" t="s">
         <v>272</v>
       </c>
-      <c r="C69" s="2" t="s">
+      <c r="D69" s="2" t="s">
         <v>273</v>
-      </c>
-      <c r="D69" s="2" t="s">
-        <v>242</v>
       </c>
       <c r="E69" s="2" t="s">
         <v>274</v>
       </c>
       <c r="F69" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A70" s="2" t="s">
-        <v>275</v>
-      </c>
-      <c r="B70" s="2" t="s">
-        <v>276</v>
-      </c>
-      <c r="C70" s="2" t="s">
-        <v>277</v>
-      </c>
-      <c r="D70" s="2" t="s">
-        <v>278</v>
-      </c>
-      <c r="E70" s="2" t="s">
-        <v>279</v>
-      </c>
-      <c r="F70" s="1">
         <v>1</v>
       </c>
     </row>

</xml_diff>